<commit_message>
Mise à jour de la dépendance annuaire et FrCore (#64)
* update deps

* generate intended recipient extension

* change file name

* rm unused aliases

* updat edeps

* adapt to new FrCore

* update status to trial-use

* correct sdemey comments

* clean urls

* update authororg sp

* update links

* update sp isArchives

* rm canonical url

* Update ig.ini ac3a46b3b827d2137e126b8fef22947f6ea3b39b
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-02T07:44:53+00:00</t>
+    <t>2024-05-03T07:57:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -647,7 +647,7 @@
     <t>isArchived</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/pdsm-is-archived}
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/pdsm-ext-is-archived}
 </t>
   </si>
   <si>
@@ -835,7 +835,7 @@
  TRE_A04-TypeDocument-LOINC, OID : 2.16.840.1.113883.6.1
  TRE_A12-NomenclatureASTM, OID : ASTM
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J66-TypeCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J07-XdsTypeCode-CISIS peut être utilisé. {f:type}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J07-XdsTypeCode-CISIS peut être utilisé. {null}</t>
   </si>
   <si>
     <t>typeDocument : [0..1] Code</t>
@@ -890,7 +890,7 @@
 -	TRE_A03-ClasseDocument-CISIS, OID : 1.2.250.1.213.1.1.4.1
 -	TRE_A10-NomenclatureURN, OID : URN
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J57-ClassCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J06-XdsClassCode-CISIS peut être utilisé. {f:category}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J06-XdsClassCode-CISIS peut être utilisé. {null}</t>
   </si>
   <si>
     <t>classeDocument : [0..1] Code</t>
@@ -914,7 +914,7 @@
     <t>DocumentReference.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://interopsante.org/fhir/StructureDefinition/FrPatient)
+    <t xml:space="preserve">Reference(https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-patient)
 </t>
   </si>
   <si>
@@ -979,7 +979,7 @@
     <t>DocumentReference.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-practitionerrole|Device|http://interopsante.org/fhir/StructureDefinition/FrPatient) &lt;&lt;contained&gt;&gt;
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-practitionerrole|Device|https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-patient) &lt;&lt;contained&gt;&gt;
 </t>
   </si>
   <si>
@@ -1092,7 +1092,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-cdr-rempl:Elément requis lorsque le flux envoyé correspond au remplacement d'un document {f:relatesTo}constr-bind-relatesTo:Cardinalité contrainte à [1..1] lorsque le flux envoyé correspond au remplacement d’un document. {f:relatesTo}</t>
+constr-cdr-rempl:Elément requis lorsque le flux envoyé correspond au remplacement d'un document {null}constr-bind-relatesTo:Cardinalité contrainte à [1..1] lorsque le flux envoyé correspond au remplacement d’un document. {null}</t>
   </si>
   <si>
     <t>Composition.relatesTo</t>
@@ -1177,7 +1177,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-bind-relatesToTarget:Référence contrainte au profil PDSm_ComprehensiveDocumentReference {f:relatesTo/f:target}</t>
+constr-bind-relatesToTarget:Référence contrainte au profil PDSm_ComprehensiveDocumentReference {null}</t>
   </si>
   <si>
     <t>idFicheAssociation : [0..*] Identifiant</t>
@@ -1239,7 +1239,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-bind-securityLabel:Les codes pour cet élément doivent provenir du ValueSet spécifié par le standard. Lorsqu’aucun code ne correspond au concept recherché, un code provenant de la terminologie de référence TRE_A07-StatusVisibiliteDocument, OID : 1.2.250.1.213.1.1.4.13 peut être utilisé. {f:securityLabel}</t>
+constr-bind-securityLabel:Les codes pour cet élément doivent provenir du ValueSet spécifié par le standard. Lorsqu’aucun code ne correspond au concept recherché, un code provenant de la terminologie de référence TRE_A07-StatusVisibiliteDocument, OID : 1.2.250.1.213.1.1.4.13 peut être utilisé. {null}</t>
   </si>
   <si>
     <t>niveauConfidentialite : [0..*] code</t>
@@ -1432,7 +1432,7 @@
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 constr-bind-attachmenturl:Dans le cas de l’ajout de document, l’url fait référence à la ressource Binary (« Binary/[id] »).
-Dans le cas de la recherche, il s’agit de l’URL permettant d’accéder au document {f:content/f:attachment/f:url}</t>
+Dans le cas de la recherche, il s’agit de l’URL permettant d’accéder au document {null}</t>
   </si>
   <si>
     <t>Document : [0..1]</t>
@@ -1573,7 +1573,7 @@
 - TRE_A09-DICOMuidRegistry, OID : 1.2.840.10008.2.6.1
 - TRE_A10-NomenclatureURN, OID : URN
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J60-FormatCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J10-XdsFormatCode-CISIS peut être utilisé. {f:content/f:format}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J10-XdsFormatCode-CISIS peut être utilisé. {null}</t>
   </si>
   <si>
     <t>formatDocument : [0..1] Code</t>
@@ -1659,7 +1659,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-constr-bind-context-event:Nomenclatures utilisées : 1) CCAM pour les actes médicaux (OID="1.2.250.1.213.2.5"); 2) CIM-10 pour les diagnostics de pathologie (OID="2.16.840.1.113883.6.3"), 3) TRE_A00-ProducteurDocNonPS pour les documents d'expression personnelle du patient, 4) autre {f:context/f:event}</t>
+constr-bind-context-event:Nomenclatures utilisées : 1) CCAM pour les actes médicaux (OID="1.2.250.1.213.2.5"); 2) CIM-10 pour les diagnostics de pathologie (OID="2.16.840.1.113883.6.3"), 3) TRE_A00-ProducteurDocNonPS pour les documents d'expression personnelle du patient, 4) autre {null}</t>
   </si>
   <si>
     <t>actePathologie : [0..1] Code</t>
@@ -1787,7 +1787,7 @@
 -	TRE_A00-ProducteurDocNonPS, OID : 1.2.250.1.213.1.1.4.6 (lorsque l’auteur du document est un patient ou un équipement sous sa responsabilité)
 -	TRE_R02-SecteurActivite, OID : 1.2.250.1.71.4.2.4 (lorsque l’auteur du document est un professionnel ou un équipement sous sa responsabilité)
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J61-HealthcareFacilityTypeCode-DMP).
-En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J02-XdsHealthcareFacilityTypeCode-CISIS peut être utilisé. {f:context/f:facilityType or f:context/f:practiceSetting}</t>
+En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J02-XdsHealthcareFacilityTypeCode-CISIS peut être utilisé. {null}</t>
   </si>
   <si>
     <t>secteurActivite : [0..1] Code</t>
@@ -1832,7 +1832,7 @@
     <t>DocumentReference.context.sourcePatientInfo</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://interopsante.org/fhir/StructureDefinition/FrPatient) &lt;&lt;contained&gt;&gt;
+    <t xml:space="preserve">Reference(https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-patient) &lt;&lt;contained&gt;&gt;
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
prepare release 3.1.0 (#69)
* prepare release 3.1.0

* add commented stu note 83902c068fda4f63e58dd7e13b700afec2064483
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.1.0-ballot</t>
+    <t>3.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-28T14:01:49+00:00</t>
+    <t>2024-05-29T09:54:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
rm TRE A04 8843c639b7005b8d3c226778368368d4683e278e
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-03T14:20:42+00:00</t>
+    <t>2024-10-31T16:32:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -838,7 +838,7 @@
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 constr-bind-type:Les valeurs possibles pour cet élément doivent provenir d’une des terminologies de référence suivantes :
  TRE_A05-TypeDocComplementaireCISIS, OID : 1.2.250.1.213.1.1.4.12
- TRE_A04-TypeDocument-LOINC, OID : 2.16.840.1.113883.6.1
+ LOINC, OID : 2.16.840.1.113883.6.1
  TRE_A12-NomenclatureASTM, OID : ASTM
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J66-TypeCode-DMP).
 En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J07-XdsTypeCode-CISIS peut être utilisé. {null}</t>

</xml_diff>

<commit_message>
Revert "rm TRE A04"
This reverts commit 8843c639b7005b8d3c226778368368d4683e278e. 4f543778be4430dbdb7ef8fc1b4d09cf7ca161ab
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/main/ig/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-31T16:32:22+00:00</t>
+    <t>2024-10-31T16:33:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -838,7 +838,7 @@
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 constr-bind-type:Les valeurs possibles pour cet élément doivent provenir d’une des terminologies de référence suivantes :
  TRE_A05-TypeDocComplementaireCISIS, OID : 1.2.250.1.213.1.1.4.12
- LOINC, OID : 2.16.840.1.113883.6.1
+ TRE_A04-TypeDocument-LOINC, OID : 2.16.840.1.113883.6.1
  TRE_A12-NomenclatureASTM, OID : ASTM
 Les valeurs possibles peuvent être restreintes en fonction du jeu de valeurs correspondant mis à disposition par le projet (exemple : JDV_J66-TypeCode-DMP).
 En l’absence de spécifications complémentaires, le jeu de valeurs JDV_J07-XdsTypeCode-CISIS peut être utilisé. {null}</t>

</xml_diff>